<commit_message>
integrating the models with backend
</commit_message>
<xml_diff>
--- a/EDA-Model/Ship_Operation_Data_Cleaned_1.xlsx
+++ b/EDA-Model/Ship_Operation_Data_Cleaned_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Ship-Operation-Systems\EDA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE3CAED-0629-46F1-A601-92D5EDBA8414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92ECC3F-1A50-4A7B-AFE9-072662F4FC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{DA5E70A5-27E7-4E8B-8F45-F65363D4431A}"/>
   </bookViews>
@@ -1120,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB53373-6E4A-4B0E-A242-10A2620AC72F}">
   <dimension ref="A1:AB1347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="U111" zoomScale="70" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>